<commit_message>
settel bahagian popup utk parliament
</commit_message>
<xml_diff>
--- a/app/dev/data/Data Parlimen Selangor.xlsx
+++ b/app/dev/data/Data Parlimen Selangor.xlsx
@@ -1,17 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\fyp\app\dev\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD1994C6-3B1C-41C2-B3D8-8BD9F6B2AF57}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="25875" windowHeight="9795"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="25875" windowHeight="9795" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
@@ -348,8 +354,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -448,6 +454,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -494,7 +508,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -526,9 +540,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -560,6 +592,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -735,16 +785,44 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:AG57"/>
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="10" width="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="8.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:33">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -845,7 +923,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:33">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>23</v>
       </c>
@@ -950,7 +1028,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:33">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="5" t="s">
         <v>28</v>
@@ -1053,7 +1131,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:33">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>30</v>
       </c>
@@ -1158,7 +1236,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:33">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
       <c r="B5" s="5" t="s">
         <v>32</v>
@@ -1261,7 +1339,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:33">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>35</v>
       </c>
@@ -1366,7 +1444,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:33">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="5" t="s">
         <v>37</v>
@@ -1469,7 +1547,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:33">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" s="9"/>
       <c r="B8" s="5" t="s">
         <v>38</v>
@@ -1572,7 +1650,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:33">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>41</v>
       </c>
@@ -1677,7 +1755,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:33">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" s="9"/>
       <c r="B10" s="5" t="s">
         <v>43</v>
@@ -1780,7 +1858,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:33">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>44</v>
       </c>
@@ -1885,7 +1963,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:33">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
       <c r="B12" s="5" t="s">
         <v>46</v>
@@ -1988,7 +2066,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:33">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>44</v>
       </c>
@@ -2093,7 +2171,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:33">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>48</v>
       </c>
@@ -2198,7 +2276,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:33">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
       <c r="B15" s="5" t="s">
         <v>50</v>
@@ -2301,7 +2379,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:33">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
       <c r="B16" s="5" t="s">
         <v>51</v>
@@ -2404,7 +2482,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:33">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>52</v>
       </c>
@@ -2509,7 +2587,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:33">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
       <c r="B18" s="5" t="s">
         <v>54</v>
@@ -2612,7 +2690,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:33">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
       <c r="B19" s="5" t="s">
         <v>55</v>
@@ -2715,7 +2793,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:33">
+    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>56</v>
       </c>
@@ -2820,7 +2898,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:33">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
       <c r="B21" s="5" t="s">
         <v>58</v>
@@ -2923,7 +3001,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:33">
+    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>59</v>
       </c>
@@ -3028,7 +3106,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:33">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
       <c r="B23" s="5" t="s">
         <v>61</v>
@@ -3131,7 +3209,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:33">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>62</v>
       </c>
@@ -3236,7 +3314,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:33">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A25" s="9"/>
       <c r="B25" s="5" t="s">
         <v>64</v>
@@ -3339,7 +3417,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:33">
+    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
       <c r="B26" s="5" t="s">
         <v>65</v>
@@ -3442,7 +3520,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:33">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>66</v>
       </c>
@@ -3547,7 +3625,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:33">
+    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A28" s="9"/>
       <c r="B28" s="5" t="s">
         <v>68</v>
@@ -3650,7 +3728,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:33">
+    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A29" s="9"/>
       <c r="B29" s="5" t="s">
         <v>69</v>
@@ -3753,7 +3831,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:33">
+    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>70</v>
       </c>
@@ -3858,7 +3936,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:33">
+    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A31" s="9"/>
       <c r="B31" s="5" t="s">
         <v>72</v>
@@ -3961,7 +4039,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:33">
+    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>73</v>
       </c>
@@ -4066,7 +4144,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:33">
+    <row r="33" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A33" s="9"/>
       <c r="B33" s="5" t="s">
         <v>75</v>
@@ -4169,7 +4247,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:33">
+    <row r="34" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>76</v>
       </c>
@@ -4274,7 +4352,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="1:33">
+    <row r="35" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A35" s="9"/>
       <c r="B35" s="5" t="s">
         <v>78</v>
@@ -4377,7 +4455,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:33">
+    <row r="36" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>79</v>
       </c>
@@ -4482,7 +4560,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="1:33">
+    <row r="37" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A37" s="9"/>
       <c r="B37" s="5" t="s">
         <v>81</v>
@@ -4585,7 +4663,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="1:33">
+    <row r="38" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>82</v>
       </c>
@@ -4690,7 +4768,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="39" spans="1:33">
+    <row r="39" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A39" s="9"/>
       <c r="B39" s="5" t="s">
         <v>84</v>
@@ -4793,7 +4871,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="40" spans="1:33">
+    <row r="40" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A40" s="9"/>
       <c r="B40" s="5" t="s">
         <v>85</v>
@@ -4896,7 +4974,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="41" spans="1:33">
+    <row r="41" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>86</v>
       </c>
@@ -5001,7 +5079,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="42" spans="1:33">
+    <row r="42" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A42" s="9"/>
       <c r="B42" s="5" t="s">
         <v>88</v>
@@ -5104,7 +5182,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="43" spans="1:33">
+    <row r="43" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>89</v>
       </c>
@@ -5209,7 +5287,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="44" spans="1:33">
+    <row r="44" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A44" s="9"/>
       <c r="B44" s="5" t="s">
         <v>91</v>
@@ -5312,7 +5390,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="45" spans="1:33">
+    <row r="45" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A45" s="9"/>
       <c r="B45" s="5" t="s">
         <v>92</v>
@@ -5415,7 +5493,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="46" spans="1:33">
+    <row r="46" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A46" s="9"/>
       <c r="B46" s="5" t="s">
         <v>93</v>
@@ -5518,7 +5596,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="47" spans="1:33">
+    <row r="47" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>94</v>
       </c>
@@ -5623,7 +5701,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="48" spans="1:33">
+    <row r="48" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A48" s="9"/>
       <c r="B48" s="5" t="s">
         <v>96</v>
@@ -5726,7 +5804,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="49" spans="1:33">
+    <row r="49" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A49" s="9"/>
       <c r="B49" s="5" t="s">
         <v>97</v>
@@ -5829,7 +5907,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="50" spans="1:33">
+    <row r="50" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>98</v>
       </c>
@@ -5934,7 +6012,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="51" spans="1:33">
+    <row r="51" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A51" s="9"/>
       <c r="B51" s="5" t="s">
         <v>100</v>
@@ -6037,7 +6115,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="52" spans="1:33">
+    <row r="52" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>101</v>
       </c>
@@ -6142,7 +6220,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="53" spans="1:33">
+    <row r="53" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A53" s="9"/>
       <c r="B53" s="5" t="s">
         <v>103</v>
@@ -6245,7 +6323,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="54" spans="1:33">
+    <row r="54" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A54" s="9"/>
       <c r="B54" s="5" t="s">
         <v>104</v>
@@ -6348,7 +6426,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="55" spans="1:33">
+    <row r="55" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>105</v>
       </c>
@@ -6453,7 +6531,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="56" spans="1:33">
+    <row r="56" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A56" s="9"/>
       <c r="B56" s="5" t="s">
         <v>107</v>
@@ -6556,7 +6634,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="57" spans="1:33">
+    <row r="57" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A57" s="9"/>
       <c r="B57" s="5" t="s">
         <v>108</v>
@@ -6665,24 +6743,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>